<commit_message>
updated arguments; using defaults
</commit_message>
<xml_diff>
--- a/inst/extdata/elisa_example_2.xlsx
+++ b/inst/extdata/elisa_example_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umassmed-my.sharepoint.com/personal/shubham_dutta_umassmed_edu/Documents/01_Personal/00_Important_main/02_R-projects/00_Packages/96_ELISA/elisa/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{A09210F2-C5C4-BC44-9E1F-8F432A59271F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09477E78-8FCB-374F-A8F3-B84DE2A4C219}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{A09210F2-C5C4-BC44-9E1F-8F432A59271F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5265D00E-2CAF-A346-889C-7B0C82ABF06C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20240" xr2:uid="{0D4292C6-5D48-844B-8CE8-B0CBAE131DFA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="69">
   <si>
     <t>A</t>
   </si>
@@ -234,9 +234,6 @@
   </si>
   <si>
     <t>coat_protein_type</t>
-  </si>
-  <si>
-    <t>coat_protein_conc</t>
   </si>
   <si>
     <t>po</t>
@@ -632,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A08853-2DAF-9A44-A0F0-AFDAD6F411B1}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:M9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,7 +640,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1012,7 +1009,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1787,7 +1784,7 @@
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
         <v>63</v>
@@ -2149,7 +2146,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2518,7 +2515,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B51">
         <v>1</v>

</xml_diff>